<commit_message>
update antiSmash ui requirement input to allow either fasta or genbank
</commit_message>
<xml_diff>
--- a/docs/UI/EDGE-v3-antiSmash-ui.xlsx
+++ b/docs/UI/EDGE-v3-antiSmash-ui.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lanl-my.sharepoint.com/personal/218819_win_lanl_gov/Documents/EDGEv3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chien-chi/Projects/LANL_git/EDGE_workflows/docs/UI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{8BC8839C-89DC-854E-9126-034D21072723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2201C376-9DFF-E543-846E-B7115F5D9B36}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B36C29-A926-B443-B2F1-BDDE80612B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22180" yWindow="4420" windowWidth="27240" windowHeight="16440" xr2:uid="{AE4FE3F8-402C-914B-AA08-CFF47FD450A1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{AE4FE3F8-402C-914B-AA08-CFF47FD450A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,15 +65,9 @@
     <t>no</t>
   </si>
   <si>
-    <t>File inputFasta</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>Input FASTA File</t>
-  </si>
-  <si>
     <t>String? smaTaxon</t>
   </si>
   <si>
@@ -180,6 +174,12 @@
   </si>
   <si>
     <t>Cluster-border prediction based on transcription factor binding sites (CASSIS)</t>
+  </si>
+  <si>
+    <t>Input FASTA/Genbank File</t>
+  </si>
+  <si>
+    <t>File inputFile</t>
   </si>
 </sst>
 </file>
@@ -557,14 +557,14 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="5" max="5" width="64.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -601,13 +601,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -615,195 +615,195 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" t="b">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" t="b">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>